<commit_message>
twilio and phone verify
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>இது முதல் கேள்வி1   
 பதில்1 பதில்2 பதில்3 பதில்4</t>
@@ -22,16 +22,30 @@
   <si>
     <t>பதில்1</t>
   </si>
+  <si>
+    <t>இது முதல் கேள்வி1   
+பதில்1 பதில்2 பதில்3 பதில்5</t>
+  </si>
+  <si>
+    <t>லோரெம் இப்சம் என்பது அச்சு மற்றும் தட்டச்சுத் துறையின் போலி உரை. லோரெம் இப்சம் 1500 களில் இருந்து தொழில்துறையின் நிலையான போலி உரையாக இருந்து வருகிறது, அப்போது ஒரு அறியப்படாத அச்சுப்பொறி ஒரு வகை மாதிரியை எடுத்து ஒரு வகை மாதிரி புத்தகத்தை உருவாக்க அதைத் துடைத்தது. இது ஐந்து நூற்றாண்டுகள் மட்டுமல்ல, மின்னணு தட்டச்சு அமைப்பிலும் பாய்ந்தது, அடிப்படையில் மாறாமல் உள்ளது. இது 1960 களில் லோரெம் இப்சம் பத்திகளைக் கொண்ட லெட்ராசெட் தாள்களை வெளியிடுவதன் மூலம் பிரபலப்படுத்தப்பட்டது, மேலும் சமீபத்தில் லோரெம் இப்ஸமின் பதிப்புகள் உட்பட ஆல்டஸ் பேஜ்மேக்கர் போன்ற டெஸ்க்டாப் வெளியீட்டு மென்பொருளுடன்.</t>
+  </si>
+  <si>
+    <t>இது முதல் கேள்வி1   
+பதில்1 பதில்2 பதில்3 பதில்21</t>
+  </si>
+  <si>
+    <t>பதில்18</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -43,22 +57,59 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -66,22 +117,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -96,9 +147,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -106,7 +157,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -116,58 +182,6 @@
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -195,25 +209,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -225,157 +353,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -386,36 +400,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -434,11 +418,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -467,6 +457,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -491,15 +505,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -509,64 +523,64 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -575,64 +589,64 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -962,16 +976,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="7" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="30.5555555555556" customWidth="1"/>
-    <col min="2" max="2" width="23.7777777777778" customWidth="1"/>
+    <col min="1" max="1" width="39.5555555555556" customWidth="1"/>
+    <col min="2" max="2" width="30.1111111111111" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="33.6" spans="1:2">
@@ -982,8 +996,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="1"/>
+    <row r="2" ht="33.6" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1"/>
@@ -1002,6 +1021,41 @@
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18" ht="33.6" spans="1:2">
+      <c r="A18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>